<commit_message>
added License file and  comments, removed a sequence
</commit_message>
<xml_diff>
--- a/SportsInviter/Data/Input/Schedule.xlsx
+++ b/SportsInviter/Data/Input/Schedule.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D07C6BB-3FB7-4825-8DF0-28300AA401E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C268587-1214-47C7-8063-2B31046CFA92}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,7 +1242,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="8">
-        <v>43638</v>
+        <v>43639</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Code ready for demo
</commit_message>
<xml_diff>
--- a/SportsInviter/Data/Input/Schedule.xlsx
+++ b/SportsInviter/Data/Input/Schedule.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C268587-1214-47C7-8063-2B31046CFA92}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26BE54E-9FB9-4B1A-B0B7-5CE0B26C7706}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1410" yWindow="1515" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="37">
   <si>
     <t>No.</t>
   </si>
@@ -582,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,6 +1260,29 @@
         <v>35</v>
       </c>
     </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="8">
+        <v>43639</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>